<commit_message>
updated weekly group update sheet
</commit_message>
<xml_diff>
--- a/Weekly Group Update Sheet.xlsx
+++ b/Weekly Group Update Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flooofy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-16.04\home\floofy\AdvProg\Assignment_2\github\AdvProg_A2_GreenDino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50A3B639-2D6C-4977-B7A7-BD62386C19BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A58635-E914-4BFC-90CF-4B5915C3CF5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0A4B5FC3-0136-B14A-9B40-3E7830ECEC8E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
   <si>
     <t>Week 7</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>Completed main menu with "credits"</t>
+  </si>
+  <si>
+    <t>Decided on where to use linkedlist/vector/array, done simple user main menu, contributed to saved-game format</t>
+  </si>
+  <si>
+    <t>Completed initial design of ADTs, linkedlist implementation, contributed to saved-game format</t>
   </si>
 </sst>
 </file>
@@ -436,16 +442,212 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -814,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB16DE-CA26-1841-81B8-0823EC851E9B}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -937,13 +1139,13 @@
       <c r="F13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="30" t="s">
+      <c r="I13" s="28" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1009,10 +1211,10 @@
       <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="29"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="11"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -1044,7 +1246,7 @@
         <v>Amy Nguyen</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
       <c r="D22" s="26" t="s">
         <v>30</v>
@@ -1053,9 +1255,15 @@
       <c r="F22" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="12"/>
+      <c r="G22" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
@@ -1066,9 +1274,15 @@
       <c r="F23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="12"/>
+      <c r="G23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
@@ -1079,9 +1293,15 @@
       <c r="F24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="12"/>
+      <c r="G24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
@@ -1118,10 +1338,10 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="30"/>
       <c r="F28" s="11"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -1224,10 +1444,10 @@
       <c r="C38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="30"/>
       <c r="F38" s="22"/>
       <c r="G38" s="23"/>
       <c r="H38" s="23"/>
@@ -1330,10 +1550,10 @@
       <c r="C48" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="28" t="s">
+      <c r="D48" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="29"/>
+      <c r="E48" s="30"/>
       <c r="F48" s="22"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -1436,10 +1656,10 @@
       <c r="C58" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D58" s="28" t="s">
+      <c r="D58" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="29"/>
+      <c r="E58" s="30"/>
       <c r="F58" s="22"/>
       <c r="G58" s="23"/>
       <c r="H58" s="23"/>
@@ -1454,20 +1674,104 @@
     <mergeCell ref="D58:E58"/>
   </mergeCells>
   <conditionalFormatting sqref="A19:XFD20 A18:D18 A29:XFD30 A28:D28 A39:XFD40 A38:D38 A49:XFD50 A48:D48 A59:XFD1048576 A58:D58 F18:XFD18 A21:E27 J21:XFD28 J31:XFD38 A41:E47 J41:XFD48 J51:XFD58 A31:E37 A51:E52 A57:E57 A53:C56 E53:E56 D54:D56 A1:XFD17">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="29" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="30" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="31" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="32" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:I28">
+  <conditionalFormatting sqref="F21:I22 F25:I28 F23:F24">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>$E$5</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updating Weekly Group Update Sheet
</commit_message>
<xml_diff>
--- a/Weekly Group Update Sheet.xlsx
+++ b/Weekly Group Update Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-16.04\home\floofy\AdvProg\Assignment_2\github\AdvProg_A2_GreenDino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aki/Documents/Uni/SEM1/APT/Assignment/A2/AdvProg_A2_GreenDino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A58635-E914-4BFC-90CF-4B5915C3CF5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44985BE0-BCE6-B94B-B513-9F44C4FAA53D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0A4B5FC3-0136-B14A-9B40-3E7830ECEC8E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" xr2:uid="{0A4B5FC3-0136-B14A-9B40-3E7830ECEC8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>Week 7</t>
   </si>
@@ -213,6 +211,18 @@
   </si>
   <si>
     <t>Completed initial design of ADTs, linkedlist implementation, contributed to saved-game format</t>
+  </si>
+  <si>
+    <t>ADT implementation for storing information is still in progress.</t>
+  </si>
+  <si>
+    <t>Implementation of linked lists, arrays and vectors where suitable. Test cases were used where necessary to test whether certain methods were working or not.</t>
+  </si>
+  <si>
+    <t>Implementation of arrays and vectors where suitable. Test cases were used where necessary to test whether certain methods were working or not.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADT implementation for storing information is still in progress. </t>
   </si>
 </sst>
 </file>
@@ -451,7 +461,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1016,11 +1082,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB16DE-CA26-1841-81B8-0823EC851E9B}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
@@ -1031,17 +1097,17 @@
     <col min="7" max="9" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -1066,7 +1132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -1077,7 +1143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
@@ -1096,7 +1162,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1170,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1196,7 @@
         <v>Amy Nguyen</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
       <c r="D13" s="26" t="s">
         <v>27</v>
@@ -1149,7 +1215,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
       <c r="D14" s="26" t="s">
         <v>28</v>
@@ -1168,7 +1234,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
       <c r="D15" s="27" t="s">
         <v>55</v>
@@ -1187,7 +1253,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
       <c r="D16" s="27" t="s">
         <v>46</v>
@@ -1198,7 +1264,7 @@
       <c r="H16" s="13"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" s="26"/>
       <c r="E17" s="12"/>
@@ -1207,7 +1273,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
@@ -1220,7 +1286,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="15"/>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>13</v>
       </c>
@@ -1246,7 +1312,7 @@
         <v>Amy Nguyen</v>
       </c>
     </row>
-    <row r="22" spans="3:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:9" ht="51" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
       <c r="D22" s="26" t="s">
         <v>30</v>
@@ -1265,7 +1331,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
       <c r="D23" s="26" t="s">
         <v>31</v>
@@ -1284,7 +1350,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
       <c r="D24" s="27" t="s">
         <v>32</v>
@@ -1303,7 +1369,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C25" s="1"/>
       <c r="D25" s="27" t="s">
         <v>39</v>
@@ -1314,7 +1380,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C26" s="1"/>
       <c r="D26" s="27" t="s">
         <v>33</v>
@@ -1325,7 +1391,7 @@
       <c r="H26" s="13"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C27" s="1"/>
       <c r="D27" s="26"/>
       <c r="E27" s="3"/>
@@ -1334,7 +1400,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
@@ -1347,7 +1413,7 @@
       <c r="H28" s="14"/>
       <c r="I28" s="15"/>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C31" s="4" t="s">
         <v>14</v>
       </c>
@@ -1360,17 +1426,20 @@
       <c r="F31" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="3:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="G31" s="4" t="str">
+        <f>$B$6</f>
+        <v>Sean Tan</v>
+      </c>
+      <c r="H31" s="5" t="str">
+        <f>$B$7</f>
+        <v>Aaron Soa</v>
+      </c>
+      <c r="I31" s="6" t="str">
+        <f>$B$8</f>
+        <v>Amy Nguyen</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" ht="68" x14ac:dyDescent="0.2">
       <c r="C32" s="1"/>
       <c r="D32" s="26" t="s">
         <v>35</v>
@@ -1379,11 +1448,17 @@
       <c r="F32" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="21"/>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="G32" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C33" s="1"/>
       <c r="D33" s="26" t="s">
         <v>38</v>
@@ -1392,11 +1467,17 @@
       <c r="F33" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="21"/>
-    </row>
-    <row r="34" spans="3:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="G33" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" ht="34" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>
       <c r="D34" s="26" t="s">
         <v>37</v>
@@ -1405,11 +1486,17 @@
       <c r="F34" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="21"/>
-    </row>
-    <row r="35" spans="3:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="G34" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" ht="34" x14ac:dyDescent="0.2">
       <c r="C35" s="1"/>
       <c r="D35" s="26" t="s">
         <v>36</v>
@@ -1420,7 +1507,7 @@
       <c r="H35" s="20"/>
       <c r="I35" s="21"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C36" s="1"/>
       <c r="D36" s="27" t="s">
         <v>34</v>
@@ -1431,7 +1518,7 @@
       <c r="H36" s="20"/>
       <c r="I36" s="21"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
       <c r="D37" s="26"/>
       <c r="E37" s="3"/>
@@ -1440,7 +1527,7 @@
       <c r="H37" s="20"/>
       <c r="I37" s="21"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C38" s="4" t="s">
         <v>1</v>
       </c>
@@ -1453,7 +1540,7 @@
       <c r="H38" s="23"/>
       <c r="I38" s="24"/>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C41" s="4" t="s">
         <v>15</v>
       </c>
@@ -1476,7 +1563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C42" s="1"/>
       <c r="D42" s="26" t="s">
         <v>44</v>
@@ -1489,7 +1576,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="21"/>
     </row>
-    <row r="43" spans="3:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:9" ht="34" x14ac:dyDescent="0.2">
       <c r="C43" s="1"/>
       <c r="D43" s="26" t="s">
         <v>40</v>
@@ -1502,7 +1589,7 @@
       <c r="H43" s="20"/>
       <c r="I43" s="21"/>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C44" s="1"/>
       <c r="D44" s="26" t="s">
         <v>43</v>
@@ -1515,7 +1602,7 @@
       <c r="H44" s="20"/>
       <c r="I44" s="21"/>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C45" s="1"/>
       <c r="D45" s="26" t="s">
         <v>48</v>
@@ -1526,7 +1613,7 @@
       <c r="H45" s="20"/>
       <c r="I45" s="21"/>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:9" ht="17" x14ac:dyDescent="0.2">
       <c r="C46" s="1"/>
       <c r="D46" s="26" t="s">
         <v>47</v>
@@ -1537,7 +1624,7 @@
       <c r="H46" s="20"/>
       <c r="I46" s="21"/>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C47" s="1"/>
       <c r="D47" s="26"/>
       <c r="E47" s="3"/>
@@ -1546,7 +1633,7 @@
       <c r="H47" s="20"/>
       <c r="I47" s="21"/>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C48" s="4" t="s">
         <v>1</v>
       </c>
@@ -1559,7 +1646,7 @@
       <c r="H48" s="23"/>
       <c r="I48" s="24"/>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C51" s="4" t="s">
         <v>16</v>
       </c>
@@ -1582,7 +1669,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C52" s="1"/>
       <c r="D52" s="2" t="s">
         <v>41</v>
@@ -1595,7 +1682,7 @@
       <c r="H52" s="20"/>
       <c r="I52" s="21"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C53" s="1"/>
       <c r="D53" t="s">
         <v>42</v>
@@ -1608,7 +1695,7 @@
       <c r="H53" s="20"/>
       <c r="I53" s="21"/>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C54" s="1"/>
       <c r="D54" s="2" t="s">
         <v>45</v>
@@ -1621,7 +1708,7 @@
       <c r="H54" s="20"/>
       <c r="I54" s="21"/>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C55" s="1"/>
       <c r="D55" s="2" t="s">
         <v>25</v>
@@ -1632,7 +1719,7 @@
       <c r="H55" s="20"/>
       <c r="I55" s="21"/>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C56" s="1"/>
       <c r="D56" s="25" t="s">
         <v>26</v>
@@ -1643,7 +1730,7 @@
       <c r="H56" s="20"/>
       <c r="I56" s="21"/>
     </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C57" s="1"/>
       <c r="D57" s="2"/>
       <c r="E57" s="3"/>
@@ -1652,7 +1739,7 @@
       <c r="H57" s="20"/>
       <c r="I57" s="21"/>
     </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C58" s="4" t="s">
         <v>1</v>
       </c>
@@ -1674,104 +1761,146 @@
     <mergeCell ref="D58:E58"/>
   </mergeCells>
   <conditionalFormatting sqref="A19:XFD20 A18:D18 A29:XFD30 A28:D28 A39:XFD40 A38:D38 A49:XFD50 A48:D48 A59:XFD1048576 A58:D58 F18:XFD18 A21:E27 J21:XFD28 J31:XFD38 A41:E47 J41:XFD48 J51:XFD58 A31:E37 A51:E52 A57:E57 A53:C56 E53:E56 D54:D56 A1:XFD17">
-    <cfRule type="cellIs" dxfId="7" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:I22 F25:I28 F23:F24">
-    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>$E$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>$E$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>$E$7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>$E$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>$E$5</formula>
     </cfRule>

</xml_diff>